<commit_message>
making morph the same
</commit_message>
<xml_diff>
--- a/test_cases/trench_test/outputs.xlsx
+++ b/test_cases/trench_test/outputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4117/Documents/PhD/adapt_utils/test_cases/trench_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB29B363-44E4-A843-BE4C-A1B88871596E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D886677-B72E-CA42-BEF1-5296E056EDC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>error</t>
   </si>
@@ -64,9 +64,6 @@
   </si>
   <si>
     <t>error to fixed</t>
-  </si>
-  <si>
-    <t>need to be re-run</t>
   </si>
 </sst>
 </file>
@@ -218,7 +215,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,12 +393,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -618,7 +609,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -629,16 +620,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1721,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1786,7 +1775,7 @@
         <v>3.2625794938779401E-2</v>
       </c>
       <c r="F3" s="7"/>
-      <c r="G3" s="11">
+      <c r="G3" s="10">
         <v>2445.9596641063599</v>
       </c>
     </row>
@@ -1798,12 +1787,14 @@
       <c r="C4" s="2">
         <v>0.3</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="14">
+        <v>4.3353741552756599E-2</v>
+      </c>
       <c r="E4" s="8">
         <v>3.7282912268870899E-2</v>
       </c>
       <c r="F4" s="8"/>
-      <c r="G4" s="12">
+      <c r="G4" s="11">
         <v>1844.9871377944901</v>
       </c>
     </row>
@@ -1822,8 +1813,8 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14" t="s">
+      <c r="G5" s="12"/>
+      <c r="H5" s="13" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1838,20 +1829,20 @@
       <c r="D6">
         <v>200</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="15">
         <v>3.0689980611109401E-2</v>
       </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16">
-        <v>3907.5375587940198</v>
+      <c r="F6" s="15"/>
+      <c r="G6" s="14">
+        <v>3147.3025443553902</v>
       </c>
       <c r="H6">
         <v>100</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="14">
         <v>3.0292410547853799E-2</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="14">
         <v>3129.18601822853</v>
       </c>
     </row>
@@ -1869,9 +1860,9 @@
       <c r="E7" s="17">
         <v>3.27705300837529E-2</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16">
-        <v>4012.9246525764402</v>
+      <c r="F7" s="15"/>
+      <c r="G7" s="14">
+        <v>3304.8026211261699</v>
       </c>
       <c r="H7">
         <v>100</v>
@@ -1888,12 +1879,18 @@
       <c r="D8">
         <v>200</v>
       </c>
-      <c r="E8" s="19">
+      <c r="E8" s="16">
         <v>3.2517797582874798E-2</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="19">
+      <c r="F8" s="15"/>
+      <c r="G8" s="16">
         <v>3348.8961756229401</v>
+      </c>
+      <c r="I8" s="14">
+        <v>3.1911495676892901E-2</v>
+      </c>
+      <c r="K8" s="14">
+        <v>3751.6653821468299</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -1910,9 +1907,9 @@
       <c r="E9" s="17">
         <v>3.2521063623563502E-2</v>
       </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16">
-        <v>4174.7958521842902</v>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14">
+        <v>3483.0631110668101</v>
       </c>
       <c r="H9">
         <v>100</v>
@@ -1932,12 +1929,18 @@
       <c r="E10" s="17">
         <v>3.2960863150087998E-2</v>
       </c>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17">
-        <v>4386.72144675254</v>
+      <c r="F10" s="15"/>
+      <c r="G10" s="14">
+        <v>3750.2131514549201</v>
       </c>
       <c r="H10">
         <v>100</v>
+      </c>
+      <c r="I10" s="14">
+        <v>3.3026483252437802E-2</v>
+      </c>
+      <c r="K10" s="14">
+        <v>3631.2981255054401</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -1955,18 +1958,73 @@
         <v>3.30058934526304E-2</v>
       </c>
       <c r="F11" s="17"/>
-      <c r="G11" s="17">
-        <v>4846.2026216983704</v>
+      <c r="G11" s="14">
+        <v>4259.0508139133399</v>
       </c>
       <c r="H11">
         <v>100</v>
       </c>
-      <c r="I11" s="10"/>
+      <c r="I11" s="14">
+        <v>3.2672974530606698E-2</v>
+      </c>
+      <c r="K11" s="14">
+        <v>4049.03709411621</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E13" s="17" t="s">
-        <v>11</v>
-      </c>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14">
+        <v>4.2946890649895597E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16" s="14">
+        <v>3.8885946849219401E-2</v>
+      </c>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>20</v>
+      </c>
+      <c r="D17" s="14">
+        <v>3.58215440050298E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>50</v>
+      </c>
+      <c r="D18" s="14">
+        <v>3.1682086124572899E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>100</v>
+      </c>
+      <c r="D19" s="14">
+        <v>3.0292410547853799E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>200</v>
+      </c>
+      <c r="D20" s="15">
+        <v>3.0689980611109401E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding beach test case
</commit_message>
<xml_diff>
--- a/test_cases/trench_test/outputs.xlsx
+++ b/test_cases/trench_test/outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mc4117/Documents/PhD/adapt_utils/test_cases/trench_test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46754E90-449B-F246-9E8E-315B0ED653EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A760363E-DFD1-9442-9D92-DD63AFACF9D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="4960" windowWidth="25600" windowHeight="14900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1100" windowWidth="25600" windowHeight="14900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="outputs" sheetId="1" r:id="rId1"/>
@@ -621,7 +621,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
@@ -632,8 +632,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1727,10 +1725,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="104" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1773,11 +1771,13 @@
         <v>0.2</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="7">
-        <v>3.2574592473285202E-2</v>
+      <c r="E2" s="12">
+        <v>3.2552451787296099E-2</v>
       </c>
       <c r="F2" s="7"/>
-      <c r="G2" s="1"/>
+      <c r="G2" s="12">
+        <v>7762.5254447460102</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1788,663 +1788,620 @@
         <v>0.3</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="7">
-        <v>3.2625794938779401E-2</v>
+      <c r="E3" s="12">
+        <v>3.2580151545557899E-2</v>
       </c>
       <c r="F3" s="7"/>
-      <c r="G3" s="10">
-        <v>2445.9596641063599</v>
+      <c r="G3" s="12">
+        <v>3229.6787159442902</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="C4" s="1">
         <v>0.3</v>
       </c>
-      <c r="D4" s="14">
-        <v>4.3353741552756599E-2</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3.7282912268870899E-2</v>
-      </c>
-      <c r="F4" s="8"/>
-      <c r="G4" s="11">
-        <v>1844.9871377944901</v>
+      <c r="D4" s="1"/>
+      <c r="E4" s="12">
+        <v>3.2016324537282002E-2</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="12">
+        <v>2933.5546991825099</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="13" t="s">
-        <v>6</v>
+      <c r="A5" s="3"/>
+      <c r="B5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="12">
+        <v>3.2847732564206797E-2</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="12">
+        <v>2734.0929727554299</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
-      <c r="B6">
-        <v>0.2</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="1">
         <v>0.3</v>
       </c>
-      <c r="D6">
-        <v>200</v>
-      </c>
-      <c r="E6" s="15">
-        <v>3.0689980611109401E-2</v>
-      </c>
-      <c r="F6" s="15"/>
-      <c r="G6" s="14">
-        <v>3147.3025443553902</v>
-      </c>
-      <c r="H6">
-        <v>100</v>
-      </c>
-      <c r="I6" s="14">
-        <v>3.0292410547853799E-2</v>
-      </c>
-      <c r="K6" s="14">
-        <v>3129.18601822853</v>
+      <c r="D6" s="1"/>
+      <c r="E6" s="12">
+        <v>3.1241974449261901E-2</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="12">
+        <v>2666.1138303279799</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0.4</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0.3</v>
       </c>
-      <c r="D7">
-        <v>200</v>
-      </c>
-      <c r="E7" s="17">
-        <v>3.27705300837529E-2</v>
-      </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="14">
-        <v>3304.8026211261699</v>
-      </c>
-      <c r="H7">
-        <v>100</v>
+      <c r="D7" s="1"/>
+      <c r="E7" s="12">
+        <v>3.0515310231200798E-2</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="12">
+        <v>2615.9116885662002</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="3"/>
-      <c r="B8">
-        <v>0.5</v>
-      </c>
-      <c r="C8">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="C8" s="2">
         <v>0.3</v>
       </c>
-      <c r="D8">
-        <v>200</v>
-      </c>
-      <c r="E8" s="16">
-        <v>3.2517797582874798E-2</v>
-      </c>
-      <c r="F8" s="15"/>
-      <c r="G8" s="16">
-        <v>3348.8961756229401</v>
-      </c>
-      <c r="I8" s="14">
-        <v>3.1911495676892901E-2</v>
-      </c>
-      <c r="K8" s="14">
-        <v>3751.6653821468299</v>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12">
+        <v>4.3970895756658003E-2</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="12">
+        <v>2484.7857148647299</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9">
-        <v>0.6</v>
-      </c>
-      <c r="C9">
-        <v>0.3</v>
-      </c>
-      <c r="D9">
-        <v>200</v>
-      </c>
-      <c r="E9" s="17">
-        <v>3.2521063623563502E-2</v>
-      </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="14">
-        <v>3483.0631110668101</v>
-      </c>
-      <c r="H9">
-        <v>100</v>
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
-      <c r="B10">
-        <v>0.8</v>
-      </c>
-      <c r="C10">
-        <v>0.3</v>
-      </c>
-      <c r="D10">
-        <v>200</v>
-      </c>
-      <c r="E10" s="17">
-        <v>3.2960863150087998E-2</v>
-      </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="14">
-        <v>3750.2131514549201</v>
-      </c>
-      <c r="H10">
-        <v>100</v>
-      </c>
-      <c r="I10" s="14">
-        <v>3.3026483252437802E-2</v>
-      </c>
-      <c r="K10" s="14">
-        <v>3631.2981255054401</v>
-      </c>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>0.3</v>
-      </c>
-      <c r="D11">
-        <v>200</v>
-      </c>
-      <c r="E11" s="17">
-        <v>3.30058934526304E-2</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="14">
-        <v>4259.0508139133399</v>
-      </c>
-      <c r="H11">
-        <v>100</v>
-      </c>
-      <c r="I11" s="14">
-        <v>3.2672974530606698E-2</v>
-      </c>
-      <c r="K11" s="14">
-        <v>4049.03709411621</v>
-      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="I12" s="12"/>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D13" s="18">
+      <c r="A13" s="3"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="K15" s="12"/>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D17" s="16">
         <v>0.2</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="G13" s="19">
+      <c r="E17" s="15"/>
+      <c r="G17" s="17">
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D14" t="s">
+    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="17" t="s">
+      <c r="E18" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G18" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H18" s="15" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15" s="20">
-        <v>4.3970896641398603E-2</v>
-      </c>
-      <c r="E15" s="22">
-        <v>7.4456203531483303E-4</v>
-      </c>
-      <c r="F15" s="21">
-        <v>3013.1972060203502</v>
-      </c>
-      <c r="G15" s="20">
-        <v>3.05153105533809E-2</v>
-      </c>
-      <c r="H15" s="22">
-        <v>1.0652812442271299E-5</v>
-      </c>
-      <c r="I15" s="21">
-        <v>3067.4686474800101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16" s="20">
-        <v>3.94933514466227E-2</v>
-      </c>
-      <c r="E16" s="22">
-        <v>5.1690405557900602E-4</v>
-      </c>
-      <c r="F16" s="21">
-        <v>3283.06614518165</v>
-      </c>
-      <c r="G16" s="20">
-        <v>3.0246997850287401E-2</v>
-      </c>
-      <c r="H16" s="22">
-        <v>1.0876126568089101E-5</v>
-      </c>
-      <c r="I16" s="21">
-        <v>3349.9419572353299</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C17">
-        <v>25</v>
-      </c>
-      <c r="D17" s="20">
-        <v>3.5302142251969003E-2</v>
-      </c>
-      <c r="E17" s="22">
-        <v>3.4358516300034498E-4</v>
-      </c>
-      <c r="F17" s="21">
-        <v>3368.83785462379</v>
-      </c>
-      <c r="G17" s="20">
-        <v>3.0400629994370099E-2</v>
-      </c>
-      <c r="H17" s="22">
-        <v>1.0309270318444401E-5</v>
-      </c>
-      <c r="I17" s="21">
-        <v>3185.3501577377301</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C18">
-        <v>50</v>
-      </c>
-      <c r="D18" s="20">
-        <v>3.22422378260886E-2</v>
-      </c>
-      <c r="E18" s="22">
-        <v>2.24439434020345E-4</v>
-      </c>
-      <c r="F18" s="21">
-        <v>3395.3445072174</v>
-      </c>
-      <c r="G18" s="20">
-        <v>3.1628820644623599E-2</v>
-      </c>
-      <c r="H18" s="22">
-        <v>1.34714808646155E-5</v>
-      </c>
-      <c r="I18" s="21">
-        <v>3519.99549365043</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C19">
-        <v>100</v>
-      </c>
-      <c r="D19" s="20">
-        <v>3.0824210452249E-2</v>
-      </c>
-      <c r="E19" s="22">
-        <v>1.39014289508364E-4</v>
-      </c>
-      <c r="F19" s="21">
-        <v>3459.6628658771501</v>
-      </c>
-      <c r="G19" s="20">
-        <v>3.2416748189123698E-2</v>
-      </c>
-      <c r="H19" s="22">
-        <v>1.80006412131551E-5</v>
-      </c>
-      <c r="I19" s="21">
-        <v>3567.7176885604799</v>
+        <v>0</v>
+      </c>
+      <c r="D19" s="18">
+        <v>4.3970896641398603E-2</v>
+      </c>
+      <c r="E19" s="20">
+        <v>7.4456203531483303E-4</v>
+      </c>
+      <c r="F19" s="19">
+        <v>3013.1972060203502</v>
+      </c>
+      <c r="G19" s="18">
+        <v>3.05153105533809E-2</v>
+      </c>
+      <c r="H19" s="20">
+        <v>1.0652812442271299E-5</v>
+      </c>
+      <c r="I19" s="19">
+        <v>3067.4686474800101</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C20">
-        <v>200</v>
-      </c>
-      <c r="D20" s="20">
-        <v>3.1074260400212099E-2</v>
-      </c>
-      <c r="E20" s="22">
-        <v>9.0153545169447294E-5</v>
-      </c>
-      <c r="F20" s="21">
-        <v>3473.2102396488099</v>
-      </c>
-      <c r="G20" s="20">
-        <v>3.2926072061808302E-2</v>
-      </c>
-      <c r="H20" s="22">
-        <v>1.57168326320592E-5</v>
-      </c>
-      <c r="I20" s="21">
-        <v>3610.0943691730499</v>
+        <v>10</v>
+      </c>
+      <c r="D20" s="18">
+        <v>3.94933514466227E-2</v>
+      </c>
+      <c r="E20" s="20">
+        <v>5.1690405557900602E-4</v>
+      </c>
+      <c r="F20" s="19">
+        <v>3283.06614518165</v>
+      </c>
+      <c r="G20" s="18">
+        <v>3.0246997850287401E-2</v>
+      </c>
+      <c r="H20" s="20">
+        <v>1.0876126568089101E-5</v>
+      </c>
+      <c r="I20" s="19">
+        <v>3349.9419572353299</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C21">
-        <v>500</v>
-      </c>
-      <c r="D21" s="20">
-        <v>3.2497284997674E-2</v>
-      </c>
-      <c r="E21" s="22">
-        <v>8.2315694696907801E-5</v>
-      </c>
-      <c r="F21" s="21">
-        <v>3466.1098542213399</v>
-      </c>
-      <c r="G21" s="20">
-        <v>3.2427851352577503E-2</v>
-      </c>
-      <c r="H21" s="22">
-        <v>6.9889504116301596E-6</v>
-      </c>
-      <c r="I21" s="21">
-        <v>3593.20992517471</v>
+        <v>25</v>
+      </c>
+      <c r="D21" s="18">
+        <v>3.5302142251969003E-2</v>
+      </c>
+      <c r="E21" s="20">
+        <v>3.4358516300034498E-4</v>
+      </c>
+      <c r="F21" s="19">
+        <v>3368.83785462379</v>
+      </c>
+      <c r="G21" s="18">
+        <v>3.0400629994370099E-2</v>
+      </c>
+      <c r="H21" s="20">
+        <v>1.0309270318444401E-5</v>
+      </c>
+      <c r="I21" s="19">
+        <v>3185.3501577377301</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="E22" s="18"/>
-      <c r="H22" s="18"/>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22" s="18">
+        <v>3.22422378260886E-2</v>
+      </c>
+      <c r="E22" s="20">
+        <v>2.24439434020345E-4</v>
+      </c>
+      <c r="F22" s="19">
+        <v>3395.3445072174</v>
+      </c>
+      <c r="G22" s="18">
+        <v>3.1628820644623599E-2</v>
+      </c>
+      <c r="H22" s="20">
+        <v>1.34714808646155E-5</v>
+      </c>
+      <c r="I22" s="19">
+        <v>3519.99549365043</v>
+      </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="D23" s="19">
-        <v>0.5</v>
-      </c>
-      <c r="E23" s="18"/>
-      <c r="G23" s="19">
-        <v>0.6</v>
-      </c>
-      <c r="H23" s="18"/>
-      <c r="J23" s="19">
-        <v>0.8</v>
-      </c>
-      <c r="M23" s="19">
-        <v>1</v>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23" s="18">
+        <v>3.0824210452249E-2</v>
+      </c>
+      <c r="E23" s="20">
+        <v>1.39014289508364E-4</v>
+      </c>
+      <c r="F23" s="19">
+        <v>3459.6628658771501</v>
+      </c>
+      <c r="G23" s="18">
+        <v>3.2416748189123698E-2</v>
+      </c>
+      <c r="H23" s="20">
+        <v>1.80006412131551E-5</v>
+      </c>
+      <c r="I23" s="19">
+        <v>3567.7176885604799</v>
       </c>
     </row>
     <row r="24" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="J24" t="s">
-        <v>11</v>
-      </c>
-      <c r="K24" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="M24" t="s">
-        <v>11</v>
-      </c>
-      <c r="N24" s="17" t="s">
-        <v>12</v>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24" s="18">
+        <v>3.1074260400212099E-2</v>
+      </c>
+      <c r="E24" s="20">
+        <v>9.0153545169447294E-5</v>
+      </c>
+      <c r="F24" s="19">
+        <v>3473.2102396488099</v>
+      </c>
+      <c r="G24" s="18">
+        <v>3.2926072061808302E-2</v>
+      </c>
+      <c r="H24" s="20">
+        <v>1.57168326320592E-5</v>
+      </c>
+      <c r="I24" s="19">
+        <v>3610.0943691730499</v>
       </c>
     </row>
     <row r="25" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25" s="20">
-        <v>3.1241974668980901E-2</v>
-      </c>
-      <c r="E25" s="22">
-        <v>6.3505666662442697E-6</v>
-      </c>
-      <c r="F25" s="21">
-        <v>3006.24324917793</v>
-      </c>
-      <c r="G25" s="20">
-        <v>3.2847732737203303E-2</v>
-      </c>
-      <c r="H25" s="22">
-        <v>9.4898065123819306E-6</v>
-      </c>
-      <c r="I25" s="21">
-        <v>3148.63579893112</v>
-      </c>
-      <c r="J25" s="20">
-        <v>3.2016321696697297E-2</v>
-      </c>
-      <c r="K25" s="20"/>
-      <c r="L25" s="21">
-        <v>3203.9936952590901</v>
-      </c>
-      <c r="M25" s="14">
-        <v>3.25801486028163E-2</v>
-      </c>
-      <c r="N25" s="20"/>
-      <c r="O25" s="14">
-        <v>3581.50642728805</v>
+        <v>500</v>
+      </c>
+      <c r="D25" s="18">
+        <v>3.2497284997674E-2</v>
+      </c>
+      <c r="E25" s="20">
+        <v>8.2315694696907801E-5</v>
+      </c>
+      <c r="F25" s="19">
+        <v>3466.1098542213399</v>
+      </c>
+      <c r="G25" s="18">
+        <v>3.2427851352577503E-2</v>
+      </c>
+      <c r="H25" s="20">
+        <v>6.9889504116301596E-6</v>
+      </c>
+      <c r="I25" s="19">
+        <v>3593.20992517471</v>
       </c>
     </row>
     <row r="26" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C26">
-        <v>10</v>
-      </c>
-      <c r="D26" s="20">
-        <v>3.1307437978153198E-2</v>
-      </c>
-      <c r="E26" s="22">
-        <v>5.8332319563773902E-6</v>
-      </c>
-      <c r="F26" s="21">
-        <v>3300.5492961406699</v>
-      </c>
-      <c r="G26" s="20">
-        <v>3.2260583608357402E-2</v>
-      </c>
-      <c r="H26" s="22">
-        <v>5.12462566477204E-6</v>
-      </c>
-      <c r="I26" s="21">
-        <v>3494.54886388778</v>
-      </c>
-      <c r="J26" s="20">
-        <v>3.19705187581776E-2</v>
-      </c>
-      <c r="K26" s="20"/>
-      <c r="L26" s="21">
-        <v>3521.1427118778201</v>
-      </c>
-      <c r="M26" s="14">
-        <v>3.2352587033207002E-2</v>
-      </c>
-      <c r="N26" s="20"/>
-      <c r="O26" s="14">
-        <v>3904.73136019706</v>
-      </c>
+      <c r="E26" s="16"/>
+      <c r="H26" s="16"/>
     </row>
     <row r="27" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C27">
-        <v>25</v>
-      </c>
-      <c r="D27" s="20">
-        <v>3.1957379569640898E-2</v>
-      </c>
-      <c r="E27" s="22">
-        <v>6.6700485536535104E-6</v>
-      </c>
-      <c r="F27" s="21">
-        <v>3423.6861763000402</v>
-      </c>
-      <c r="G27" s="20">
-        <v>3.2033752134803299E-2</v>
-      </c>
-      <c r="H27" s="22">
-        <v>3.7814091792849502E-6</v>
-      </c>
-      <c r="I27" s="21">
-        <v>3549.4822981357502</v>
-      </c>
-      <c r="J27" s="20">
-        <v>3.2291859161858998E-2</v>
-      </c>
-      <c r="K27" s="20"/>
-      <c r="L27" s="21">
-        <v>3620.62393450737</v>
-      </c>
-      <c r="M27" s="14">
-        <v>3.2385095440773802E-2</v>
-      </c>
-      <c r="N27" s="20"/>
-      <c r="O27" s="14">
-        <v>3966.69863772392</v>
+      <c r="D27" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="16"/>
+      <c r="G27" s="17">
+        <v>0.6</v>
+      </c>
+      <c r="H27" s="16"/>
+      <c r="J27" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="M27" s="17">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="3:15" x14ac:dyDescent="0.2">
-      <c r="C28">
-        <v>50</v>
-      </c>
-      <c r="D28" s="20">
-        <v>3.1122295250174899E-2</v>
-      </c>
-      <c r="E28" s="22">
-        <v>4.7148934179992597E-6</v>
-      </c>
-      <c r="F28" s="21">
-        <v>3517.0594332218102</v>
-      </c>
-      <c r="G28" s="20">
-        <v>3.23762275366676E-2</v>
-      </c>
-      <c r="H28" s="22">
-        <v>4.7860869589128501E-6</v>
-      </c>
-      <c r="I28" s="21">
-        <v>3599.2063477039301</v>
-      </c>
-      <c r="J28" s="20">
-        <v>3.2425046226593202E-2</v>
-      </c>
-      <c r="L28" s="21">
-        <v>3657.6101202964701</v>
-      </c>
-      <c r="M28" s="14">
-        <v>3.2648045732106702E-2</v>
-      </c>
-      <c r="O28" s="14">
-        <v>4098.5477344989704</v>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="J28" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="M28" t="s">
+        <v>11</v>
+      </c>
+      <c r="N28" s="15" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C29">
-        <v>100</v>
-      </c>
-      <c r="D29" s="20">
-        <v>3.1781734715764703E-2</v>
-      </c>
-      <c r="E29" s="22">
-        <v>4.1237090441071998E-6</v>
-      </c>
-      <c r="F29" s="21">
-        <v>3506.2300231456702</v>
-      </c>
-      <c r="G29" s="20">
-        <v>3.2196502252235901E-2</v>
-      </c>
-      <c r="H29" s="22">
-        <v>2.3337535730752E-6</v>
-      </c>
-      <c r="I29" s="21">
-        <v>3657.9331853389699</v>
-      </c>
-      <c r="J29" s="20">
-        <v>3.3101263398379203E-2</v>
-      </c>
-      <c r="L29" s="21">
-        <v>3753.6492176055899</v>
-      </c>
-      <c r="M29" s="14">
-        <v>3.2734363118435E-2</v>
-      </c>
-      <c r="O29" s="14">
-        <v>4214.2364480495398</v>
+        <v>0</v>
+      </c>
+      <c r="D29" s="18">
+        <v>3.1241974668980901E-2</v>
+      </c>
+      <c r="E29" s="20">
+        <v>6.3505666662442697E-6</v>
+      </c>
+      <c r="F29" s="19">
+        <v>3006.24324917793</v>
+      </c>
+      <c r="G29" s="18">
+        <v>3.2847732737203303E-2</v>
+      </c>
+      <c r="H29" s="20">
+        <v>9.4898065123819306E-6</v>
+      </c>
+      <c r="I29" s="19">
+        <v>3148.63579893112</v>
+      </c>
+      <c r="J29" s="18">
+        <v>3.2016321696697297E-2</v>
+      </c>
+      <c r="K29" s="18"/>
+      <c r="L29" s="19">
+        <v>3203.9936952590901</v>
+      </c>
+      <c r="M29" s="12">
+        <v>3.25801486028163E-2</v>
+      </c>
+      <c r="N29" s="18"/>
+      <c r="O29" s="12">
+        <v>3581.50642728805</v>
       </c>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C30">
-        <v>200</v>
-      </c>
-      <c r="D30" s="20">
-        <v>3.2608526038490501E-2</v>
-      </c>
-      <c r="E30" s="22">
-        <v>5.6937535898613399E-6</v>
-      </c>
-      <c r="F30" s="21">
-        <v>3540.3143949508599</v>
-      </c>
-      <c r="G30" s="20">
-        <v>3.2635327138729499E-2</v>
-      </c>
-      <c r="H30" s="22">
-        <v>2.50670784803482E-6</v>
-      </c>
-      <c r="I30" s="21">
-        <v>3726.8867208957599</v>
-      </c>
-      <c r="J30" s="20">
-        <v>3.3035537790165402E-2</v>
-      </c>
-      <c r="K30" s="20"/>
-      <c r="L30" s="21">
-        <v>3822.9466784000301</v>
-      </c>
-      <c r="M30" s="14">
-        <v>3.3069016685497298E-2</v>
-      </c>
-      <c r="N30" s="20"/>
-      <c r="O30" s="14">
-        <v>4391.8045840263303</v>
+        <v>10</v>
+      </c>
+      <c r="D30" s="18">
+        <v>3.1307437978153198E-2</v>
+      </c>
+      <c r="E30" s="20">
+        <v>5.8332319563773902E-6</v>
+      </c>
+      <c r="F30" s="19">
+        <v>3300.5492961406699</v>
+      </c>
+      <c r="G30" s="18">
+        <v>3.2260583608357402E-2</v>
+      </c>
+      <c r="H30" s="20">
+        <v>5.12462566477204E-6</v>
+      </c>
+      <c r="I30" s="19">
+        <v>3494.54886388778</v>
+      </c>
+      <c r="J30" s="18">
+        <v>3.19705187581776E-2</v>
+      </c>
+      <c r="K30" s="18"/>
+      <c r="L30" s="19">
+        <v>3521.1427118778201</v>
+      </c>
+      <c r="M30" s="12">
+        <v>3.2352587033207002E-2</v>
+      </c>
+      <c r="N30" s="18"/>
+      <c r="O30" s="12">
+        <v>3904.73136019706</v>
       </c>
     </row>
     <row r="31" spans="3:15" x14ac:dyDescent="0.2">
       <c r="C31">
+        <v>25</v>
+      </c>
+      <c r="D31" s="18">
+        <v>3.1957379569640898E-2</v>
+      </c>
+      <c r="E31" s="20">
+        <v>6.6700485536535104E-6</v>
+      </c>
+      <c r="F31" s="19">
+        <v>3423.6861763000402</v>
+      </c>
+      <c r="G31" s="18">
+        <v>3.2033752134803299E-2</v>
+      </c>
+      <c r="H31" s="20">
+        <v>3.7814091792849502E-6</v>
+      </c>
+      <c r="I31" s="19">
+        <v>3549.4822981357502</v>
+      </c>
+      <c r="J31" s="18">
+        <v>3.2291859161858998E-2</v>
+      </c>
+      <c r="K31" s="18"/>
+      <c r="L31" s="19">
+        <v>3620.62393450737</v>
+      </c>
+      <c r="M31" s="12">
+        <v>3.2385095440773802E-2</v>
+      </c>
+      <c r="N31" s="18"/>
+      <c r="O31" s="12">
+        <v>3966.69863772392</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>50</v>
+      </c>
+      <c r="D32" s="18">
+        <v>3.1122295250174899E-2</v>
+      </c>
+      <c r="E32" s="20">
+        <v>4.7148934179992597E-6</v>
+      </c>
+      <c r="F32" s="19">
+        <v>3517.0594332218102</v>
+      </c>
+      <c r="G32" s="18">
+        <v>3.23762275366676E-2</v>
+      </c>
+      <c r="H32" s="20">
+        <v>4.7860869589128501E-6</v>
+      </c>
+      <c r="I32" s="19">
+        <v>3599.2063477039301</v>
+      </c>
+      <c r="J32" s="18">
+        <v>3.2425046226593202E-2</v>
+      </c>
+      <c r="L32" s="19">
+        <v>3657.6101202964701</v>
+      </c>
+      <c r="M32" s="12">
+        <v>3.2648045732106702E-2</v>
+      </c>
+      <c r="O32" s="12">
+        <v>4098.5477344989704</v>
+      </c>
+    </row>
+    <row r="33" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33" s="18">
+        <v>3.1781734715764703E-2</v>
+      </c>
+      <c r="E33" s="20">
+        <v>4.1237090441071998E-6</v>
+      </c>
+      <c r="F33" s="19">
+        <v>3506.2300231456702</v>
+      </c>
+      <c r="G33" s="18">
+        <v>3.2196502252235901E-2</v>
+      </c>
+      <c r="H33" s="20">
+        <v>2.3337535730752E-6</v>
+      </c>
+      <c r="I33" s="19">
+        <v>3657.9331853389699</v>
+      </c>
+      <c r="J33" s="18">
+        <v>3.3101263398379203E-2</v>
+      </c>
+      <c r="L33" s="19">
+        <v>3753.6492176055899</v>
+      </c>
+      <c r="M33" s="12">
+        <v>3.2734363118435E-2</v>
+      </c>
+      <c r="O33" s="12">
+        <v>4214.2364480495398</v>
+      </c>
+    </row>
+    <row r="34" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>200</v>
+      </c>
+      <c r="D34" s="18">
+        <v>3.2608526038490501E-2</v>
+      </c>
+      <c r="E34" s="20">
+        <v>5.6937535898613399E-6</v>
+      </c>
+      <c r="F34" s="19">
+        <v>3540.3143949508599</v>
+      </c>
+      <c r="G34" s="18">
+        <v>3.2635327138729499E-2</v>
+      </c>
+      <c r="H34" s="20">
+        <v>2.50670784803482E-6</v>
+      </c>
+      <c r="I34" s="19">
+        <v>3726.8867208957599</v>
+      </c>
+      <c r="J34" s="18">
+        <v>3.3035537790165402E-2</v>
+      </c>
+      <c r="K34" s="18"/>
+      <c r="L34" s="19">
+        <v>3822.9466784000301</v>
+      </c>
+      <c r="M34" s="12">
+        <v>3.3069016685497298E-2</v>
+      </c>
+      <c r="N34" s="18"/>
+      <c r="O34" s="12">
+        <v>4391.8045840263303</v>
+      </c>
+    </row>
+    <row r="35" spans="3:15" x14ac:dyDescent="0.2">
+      <c r="C35">
         <v>500</v>
       </c>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="21"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="21"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="19"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>